<commit_message>
Final commit with finished tasks
</commit_message>
<xml_diff>
--- a/Wholesale customers data.xlsx
+++ b/Wholesale customers data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3906\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1b86\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B7BD160-06BD-4F2F-B9C7-875947AF95E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C521A85-0F88-49E5-B429-234933B58339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>